<commit_message>
After Haunting Mars 7
</commit_message>
<xml_diff>
--- a/haunting_mars/empower_connect.xlsx
+++ b/haunting_mars/empower_connect.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dare/Documents/personal/rpg/posthuman/haunting_mars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92670CC1-A2F5-3B40-8E3E-0AB40F985969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36E99CF-5FE4-1142-98EB-4E515B886C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{418C9B73-ED0B-9E4C-958F-0A86C3A4E7F4}"/>
+    <workbookView xWindow="2240" yWindow="1500" windowWidth="28040" windowHeight="18820" xr2:uid="{418C9B73-ED0B-9E4C-958F-0A86C3A4E7F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -222,6 +222,105 @@
   </si>
   <si>
     <t>Eileen Weiss</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Imperial Aria</t>
+  </si>
+  <si>
+    <t>Wanda Eagal</t>
+  </si>
+  <si>
+    <t>Organiser</t>
+  </si>
+  <si>
+    <t>DDBS 11</t>
+  </si>
+  <si>
+    <t>Sirenum 0</t>
+  </si>
+  <si>
+    <t>Sirenum -1</t>
+  </si>
+  <si>
+    <t>Jungle in a Bottle</t>
+  </si>
+  <si>
+    <t>Stellar Intelligence</t>
+  </si>
+  <si>
+    <t>totalitarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Previously Seen</t>
+  </si>
+  <si>
+    <t>Akemi Tanizaki</t>
+  </si>
+  <si>
+    <t>Paolo Chanrdasekhar</t>
+  </si>
+  <si>
+    <t>Martian Rangers</t>
+  </si>
+  <si>
+    <t>contrarian</t>
+  </si>
+  <si>
+    <t>Haunting Mars 5</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Pontes</t>
+  </si>
+  <si>
+    <t>Elysium</t>
+  </si>
+  <si>
+    <t>Valles</t>
+  </si>
+  <si>
+    <t>Xiphos</t>
+  </si>
+  <si>
+    <t>Pavonis</t>
+  </si>
+  <si>
+    <t>Argoed</t>
+  </si>
+  <si>
+    <t>Melas</t>
+  </si>
+  <si>
+    <t>Portmanteau</t>
+  </si>
+  <si>
+    <t>Radennitia</t>
+  </si>
+  <si>
+    <t>KLH</t>
+  </si>
+  <si>
+    <t>Eddie</t>
+  </si>
+  <si>
+    <t>Octavia, Venus</t>
+  </si>
+  <si>
+    <t>Nahuatl</t>
+  </si>
+  <si>
+    <t>Haunting Mars bgr</t>
+  </si>
+  <si>
+    <t>Olympian</t>
   </si>
 </sst>
 </file>
@@ -601,19 +700,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EEA52C-16A0-4E41-812A-01FDEB790E17}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,499 +725,772 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="H1" s="1" t="str">
+        <f>"Pic ("&amp;COUNTIF(H2:H99,"x")&amp;")"</f>
+        <v>Pic (25)</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>-2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F10" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10">
-        <v>-1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12">
+        <v>-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11">
-        <v>-2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12">
-        <v>-2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>17</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16">
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18">
+        <v>-2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E19" t="s">
         <v>17</v>
       </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
       <c r="B20" t="s">
         <v>50</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>5</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21">
+      <c r="H20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24">
+        <v>-1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
         <v>5</v>
       </c>
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28">
+        <v>-2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="H28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s">
         <v>58</v>
       </c>
-      <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
         <v>18</v>
       </c>
-      <c r="F24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" t="s">
-        <v>46</v>
+      <c r="G29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J28">
+    <sortCondition ref="A2:A28"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>